<commit_message>
Update: Add more Functionality
</commit_message>
<xml_diff>
--- a/SOURCE.xlsx
+++ b/SOURCE.xlsx
@@ -1926,7 +1926,7 @@
     <t xml:space="preserve">SDN KEPATIHAN 06</t>
   </si>
   <si>
-    <t xml:space="preserve">REHAB AULA UPTD SATDIK SDN KEPATIH 06</t>
+    <t xml:space="preserve">REHAB AULA SDN KEPATIH 06</t>
   </si>
   <si>
     <t xml:space="preserve">SDN MANGLI 03</t>
@@ -2391,187 +2391,187 @@
     <t>SMP</t>
   </si>
   <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 5 SILO</t>
+    <t xml:space="preserve">SMPN 5 SILO</t>
   </si>
   <si>
     <t xml:space="preserve">Data Bidang Smp</t>
   </si>
   <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 2 MAYANG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 SUMBERBARU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 3 SUMBERJAMBE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 PAKUSARI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 3 SILO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 LEDOKOMBO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 AMBULU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 BALUNG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 13 JEMBER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 14 JEMBER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 7 JEMBER </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 8 JEMBER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 MAYANG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 4 KALISAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK  SMPN 3 PUGER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 4 SUMBERJAMBE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 2 MUMBULSARI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 4 SILO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 3 KALISAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 2 TEMPUREJO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 3 AMBULU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 4 SUKOWONO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 3 ARJASA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 4 BANGSALSARI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 SILO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 4 TEMPUREJO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 6 TANGGUL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 2 KENCONG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 2 SILO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 PUGER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 SEMBORO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 PANTI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 4 TANGGUL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 JELBUK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 JENGGAWAH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 AJUNG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 12 JEMBER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 UMBULSARI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 GUMUKMAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 2 ARJASA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 RAMBIPUJI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 BANGSALSARI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 2 BALUNG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK  SMPN 2 TANGGUL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 TANGGUL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 2 RAMBIPUJI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 WULUHAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 KALISAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 3 TANGGUL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 2 AMBULU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 2 PUGER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 4 JEMBER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 KENCONG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 MUMBULSARI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 11 JEMBER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 5 JEMBER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 2 KALISAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 2 SUKOWONO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPTD SATDIK SMPN 1 JOMBANG</t>
+    <t xml:space="preserve">SMPN 2 MAYANG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 SUMBERBARU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 3 SUMBERJAMBE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 PAKUSARI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 3 SILO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 LEDOKOMBO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 AMBULU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 BALUNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 13 JEMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 14 JEMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 7 JEMBER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 8 JEMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 MAYANG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 4 KALISAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SMPN 3 PUGER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 4 SUMBERJAMBE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 2 MUMBULSARI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 4 SILO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 3 KALISAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 2 TEMPUREJO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 3 AMBULU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 4 SUKOWONO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 3 ARJASA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 4 BANGSALSARI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 SILO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 4 TEMPUREJO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 6 TANGGUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 2 KENCONG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 2 SILO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 PUGER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 SEMBORO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 PANTI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 4 TANGGUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 JELBUK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 JENGGAWAH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 AJUNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 12 JEMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 UMBULSARI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 GUMUKMAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 2 ARJASA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 RAMBIPUJI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 BANGSALSARI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 2 BALUNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SMPN 2 TANGGUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 TANGGUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 2 RAMBIPUJI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 WULUHAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 KALISAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 3 TANGGUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 2 AMBULU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 2 PUGER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 4 JEMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 KENCONG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 MUMBULSARI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 11 JEMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 5 JEMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 2 KALISAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 2 SUKOWONO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMPN 1 JOMBANG</t>
   </si>
 </sst>
 </file>
@@ -3115,7 +3115,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A149" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -60201,7 +60201,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>